<commit_message>
code updates & data
</commit_message>
<xml_diff>
--- a/Code/Photologic Rig Main Application Code/experiment schedule.xlsx
+++ b/Code/Photologic Rig Main Application Code/experiment schedule.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:J31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -494,67 +494,1075 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>water</t>
+          <t>sucrose</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>lemon</t>
+          <t>sucrose</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>0</v>
+        <v>49</v>
       </c>
       <c r="F2" t="n">
-        <v>35</v>
+        <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>30000</v>
+        <v>20000</v>
       </c>
       <c r="H2" t="n">
-        <v>15000</v>
+        <v>10000</v>
       </c>
       <c r="I2" t="n">
-        <v>15000</v>
+        <v>10000</v>
       </c>
       <c r="J2" t="n">
-        <v>985.2156639099121</v>
+        <v>5913.367509841919</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3" t="n">
         <v>2</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>lemon</t>
+          <t>sucrose</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>water</t>
+          <t>sucrose</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>0</v>
+        <v>62</v>
       </c>
       <c r="F3" t="n">
         <v>0</v>
       </c>
       <c r="G3" t="n">
-        <v>30000</v>
+        <v>20000</v>
       </c>
       <c r="H3" t="n">
-        <v>15000</v>
+        <v>10000</v>
       </c>
       <c r="I3" t="n">
-        <v>15000</v>
+        <v>10000</v>
       </c>
       <c r="J3" t="n">
-        <v>15000</v>
+        <v>756.8745613098145</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="n">
+        <v>3</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>sucrose</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>sucrose</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
+        <v>63</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" t="n">
+        <v>20000</v>
+      </c>
+      <c r="H4" t="n">
+        <v>10000</v>
+      </c>
+      <c r="I4" t="n">
+        <v>10000</v>
+      </c>
+      <c r="J4" t="n">
+        <v>3583.076477050781</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="n">
+        <v>4</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>sucrose</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>sucrose</t>
+        </is>
+      </c>
+      <c r="E5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" t="n">
+        <v>3</v>
+      </c>
+      <c r="G5" t="n">
+        <v>20000</v>
+      </c>
+      <c r="H5" t="n">
+        <v>10000</v>
+      </c>
+      <c r="I5" t="n">
+        <v>10000</v>
+      </c>
+      <c r="J5" t="n">
+        <v>3336.502075195312</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="n">
+        <v>5</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>sucrose</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>sucrose</t>
+        </is>
+      </c>
+      <c r="E6" t="n">
+        <v>58</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0</v>
+      </c>
+      <c r="G6" t="n">
+        <v>20000</v>
+      </c>
+      <c r="H6" t="n">
+        <v>10000</v>
+      </c>
+      <c r="I6" t="n">
+        <v>10000</v>
+      </c>
+      <c r="J6" t="n">
+        <v>5307.537317276001</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="n">
+        <v>6</v>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>sucrose</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>sucrose</t>
+        </is>
+      </c>
+      <c r="E7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" t="n">
+        <v>20</v>
+      </c>
+      <c r="G7" t="n">
+        <v>20000</v>
+      </c>
+      <c r="H7" t="n">
+        <v>10000</v>
+      </c>
+      <c r="I7" t="n">
+        <v>10000</v>
+      </c>
+      <c r="J7" t="n">
+        <v>7521.06237411499</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" t="n">
+        <v>7</v>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>sucrose</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>sucrose</t>
+        </is>
+      </c>
+      <c r="E8" t="n">
+        <v>0</v>
+      </c>
+      <c r="F8" t="n">
+        <v>38</v>
+      </c>
+      <c r="G8" t="n">
+        <v>20000</v>
+      </c>
+      <c r="H8" t="n">
+        <v>10000</v>
+      </c>
+      <c r="I8" t="n">
+        <v>10000</v>
+      </c>
+      <c r="J8" t="n">
+        <v>1217.240571975708</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" t="n">
+        <v>8</v>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>sucrose</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>sucrose</t>
+        </is>
+      </c>
+      <c r="E9" t="n">
+        <v>0</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0</v>
+      </c>
+      <c r="G9" t="n">
+        <v>20000</v>
+      </c>
+      <c r="H9" t="n">
+        <v>10000</v>
+      </c>
+      <c r="I9" t="n">
+        <v>10000</v>
+      </c>
+      <c r="J9" t="n">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" t="n">
+        <v>9</v>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>sucrose</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>sucrose</t>
+        </is>
+      </c>
+      <c r="E10" t="n">
+        <v>63</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0</v>
+      </c>
+      <c r="G10" t="n">
+        <v>20000</v>
+      </c>
+      <c r="H10" t="n">
+        <v>10000</v>
+      </c>
+      <c r="I10" t="n">
+        <v>10000</v>
+      </c>
+      <c r="J10" t="n">
+        <v>3937.018871307373</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" t="n">
+        <v>10</v>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>sucrose</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>sucrose</t>
+        </is>
+      </c>
+      <c r="E11" t="n">
+        <v>0</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0</v>
+      </c>
+      <c r="G11" t="n">
+        <v>20000</v>
+      </c>
+      <c r="H11" t="n">
+        <v>10000</v>
+      </c>
+      <c r="I11" t="n">
+        <v>10000</v>
+      </c>
+      <c r="J11" t="n">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" t="n">
+        <v>11</v>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>sucrose</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>sucrose</t>
+        </is>
+      </c>
+      <c r="E12" t="n">
+        <v>0</v>
+      </c>
+      <c r="F12" t="n">
+        <v>30</v>
+      </c>
+      <c r="G12" t="n">
+        <v>20000</v>
+      </c>
+      <c r="H12" t="n">
+        <v>10000</v>
+      </c>
+      <c r="I12" t="n">
+        <v>10000</v>
+      </c>
+      <c r="J12" t="n">
+        <v>438.5979175567627</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" t="n">
+        <v>12</v>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>sucrose</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>sucrose</t>
+        </is>
+      </c>
+      <c r="E13" t="n">
+        <v>0</v>
+      </c>
+      <c r="F13" t="n">
+        <v>65</v>
+      </c>
+      <c r="G13" t="n">
+        <v>20000</v>
+      </c>
+      <c r="H13" t="n">
+        <v>10000</v>
+      </c>
+      <c r="I13" t="n">
+        <v>10000</v>
+      </c>
+      <c r="J13" t="n">
+        <v>332.0422172546387</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" t="n">
+        <v>13</v>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>sucrose</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>sucrose</t>
+        </is>
+      </c>
+      <c r="E14" t="n">
+        <v>59</v>
+      </c>
+      <c r="F14" t="n">
+        <v>0</v>
+      </c>
+      <c r="G14" t="n">
+        <v>20000</v>
+      </c>
+      <c r="H14" t="n">
+        <v>10000</v>
+      </c>
+      <c r="I14" t="n">
+        <v>10000</v>
+      </c>
+      <c r="J14" t="n">
+        <v>781.9030284881592</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" t="n">
+        <v>14</v>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>sucrose</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>sucrose</t>
+        </is>
+      </c>
+      <c r="E15" t="n">
+        <v>0</v>
+      </c>
+      <c r="F15" t="n">
+        <v>62</v>
+      </c>
+      <c r="G15" t="n">
+        <v>20000</v>
+      </c>
+      <c r="H15" t="n">
+        <v>10000</v>
+      </c>
+      <c r="I15" t="n">
+        <v>10000</v>
+      </c>
+      <c r="J15" t="n">
+        <v>997.8280067443848</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" t="n">
+        <v>15</v>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>sucrose</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>sucrose</t>
+        </is>
+      </c>
+      <c r="E16" t="n">
+        <v>61</v>
+      </c>
+      <c r="F16" t="n">
+        <v>0</v>
+      </c>
+      <c r="G16" t="n">
+        <v>20000</v>
+      </c>
+      <c r="H16" t="n">
+        <v>10000</v>
+      </c>
+      <c r="I16" t="n">
+        <v>10000</v>
+      </c>
+      <c r="J16" t="n">
+        <v>1097.296476364136</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" t="n">
+        <v>16</v>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>sucrose</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>sucrose</t>
+        </is>
+      </c>
+      <c r="E17" t="n">
+        <v>63</v>
+      </c>
+      <c r="F17" t="n">
+        <v>0</v>
+      </c>
+      <c r="G17" t="n">
+        <v>20000</v>
+      </c>
+      <c r="H17" t="n">
+        <v>10000</v>
+      </c>
+      <c r="I17" t="n">
+        <v>10000</v>
+      </c>
+      <c r="J17" t="n">
+        <v>407.6828956604004</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" t="n">
+        <v>17</v>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>sucrose</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>sucrose</t>
+        </is>
+      </c>
+      <c r="E18" t="n">
+        <v>62</v>
+      </c>
+      <c r="F18" t="n">
+        <v>0</v>
+      </c>
+      <c r="G18" t="n">
+        <v>20000</v>
+      </c>
+      <c r="H18" t="n">
+        <v>10000</v>
+      </c>
+      <c r="I18" t="n">
+        <v>10000</v>
+      </c>
+      <c r="J18" t="n">
+        <v>1176.933288574219</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" t="n">
+        <v>18</v>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>sucrose</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>sucrose</t>
+        </is>
+      </c>
+      <c r="E19" t="n">
+        <v>54</v>
+      </c>
+      <c r="F19" t="n">
+        <v>0</v>
+      </c>
+      <c r="G19" t="n">
+        <v>20000</v>
+      </c>
+      <c r="H19" t="n">
+        <v>10000</v>
+      </c>
+      <c r="I19" t="n">
+        <v>10000</v>
+      </c>
+      <c r="J19" t="n">
+        <v>830.8696746826172</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" t="n">
+        <v>19</v>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>sucrose</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>sucrose</t>
+        </is>
+      </c>
+      <c r="E20" t="n">
+        <v>0</v>
+      </c>
+      <c r="F20" t="n">
+        <v>53</v>
+      </c>
+      <c r="G20" t="n">
+        <v>20000</v>
+      </c>
+      <c r="H20" t="n">
+        <v>10000</v>
+      </c>
+      <c r="I20" t="n">
+        <v>10000</v>
+      </c>
+      <c r="J20" t="n">
+        <v>2326.441526412964</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" t="n">
+        <v>20</v>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>sucrose</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>sucrose</t>
+        </is>
+      </c>
+      <c r="E21" t="n">
+        <v>0</v>
+      </c>
+      <c r="F21" t="n">
+        <v>70</v>
+      </c>
+      <c r="G21" t="n">
+        <v>20000</v>
+      </c>
+      <c r="H21" t="n">
+        <v>10000</v>
+      </c>
+      <c r="I21" t="n">
+        <v>10000</v>
+      </c>
+      <c r="J21" t="n">
+        <v>424.4704246520996</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" t="n">
+        <v>21</v>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>sucrose</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>sucrose</t>
+        </is>
+      </c>
+      <c r="E22" t="n">
+        <v>0</v>
+      </c>
+      <c r="F22" t="n">
+        <v>68</v>
+      </c>
+      <c r="G22" t="n">
+        <v>20000</v>
+      </c>
+      <c r="H22" t="n">
+        <v>10000</v>
+      </c>
+      <c r="I22" t="n">
+        <v>10000</v>
+      </c>
+      <c r="J22" t="n">
+        <v>1157.277345657349</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>22</v>
+      </c>
+      <c r="B23" t="n">
+        <v>22</v>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>sucrose</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>sucrose</t>
+        </is>
+      </c>
+      <c r="E23" t="n">
+        <v>57</v>
+      </c>
+      <c r="F23" t="n">
+        <v>0</v>
+      </c>
+      <c r="G23" t="n">
+        <v>20000</v>
+      </c>
+      <c r="H23" t="n">
+        <v>10000</v>
+      </c>
+      <c r="I23" t="n">
+        <v>10000</v>
+      </c>
+      <c r="J23" t="n">
+        <v>2556.679964065552</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>23</v>
+      </c>
+      <c r="B24" t="n">
+        <v>23</v>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>sucrose</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>sucrose</t>
+        </is>
+      </c>
+      <c r="E24" t="n">
+        <v>65</v>
+      </c>
+      <c r="F24" t="n">
+        <v>0</v>
+      </c>
+      <c r="G24" t="n">
+        <v>20000</v>
+      </c>
+      <c r="H24" t="n">
+        <v>10000</v>
+      </c>
+      <c r="I24" t="n">
+        <v>10000</v>
+      </c>
+      <c r="J24" t="n">
+        <v>592.5307273864746</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>24</v>
+      </c>
+      <c r="B25" t="n">
+        <v>24</v>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>sucrose</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>sucrose</t>
+        </is>
+      </c>
+      <c r="E25" t="n">
+        <v>63</v>
+      </c>
+      <c r="F25" t="n">
+        <v>0</v>
+      </c>
+      <c r="G25" t="n">
+        <v>20000</v>
+      </c>
+      <c r="H25" t="n">
+        <v>10000</v>
+      </c>
+      <c r="I25" t="n">
+        <v>10000</v>
+      </c>
+      <c r="J25" t="n">
+        <v>578.0105590820312</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>25</v>
+      </c>
+      <c r="B26" t="n">
+        <v>25</v>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>sucrose</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>sucrose</t>
+        </is>
+      </c>
+      <c r="E26" t="n">
+        <v>61</v>
+      </c>
+      <c r="F26" t="n">
+        <v>0</v>
+      </c>
+      <c r="G26" t="n">
+        <v>20000</v>
+      </c>
+      <c r="H26" t="n">
+        <v>10000</v>
+      </c>
+      <c r="I26" t="n">
+        <v>10000</v>
+      </c>
+      <c r="J26" t="n">
+        <v>2439.763784408569</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>26</v>
+      </c>
+      <c r="B27" t="n">
+        <v>26</v>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>sucrose</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>sucrose</t>
+        </is>
+      </c>
+      <c r="E27" t="n">
+        <v>0</v>
+      </c>
+      <c r="F27" t="n">
+        <v>41</v>
+      </c>
+      <c r="G27" t="n">
+        <v>20000</v>
+      </c>
+      <c r="H27" t="n">
+        <v>10000</v>
+      </c>
+      <c r="I27" t="n">
+        <v>10000</v>
+      </c>
+      <c r="J27" t="n">
+        <v>1475.422620773315</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>27</v>
+      </c>
+      <c r="B28" t="n">
+        <v>27</v>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>sucrose</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>sucrose</t>
+        </is>
+      </c>
+      <c r="E28" t="n">
+        <v>58</v>
+      </c>
+      <c r="F28" t="n">
+        <v>0</v>
+      </c>
+      <c r="G28" t="n">
+        <v>20000</v>
+      </c>
+      <c r="H28" t="n">
+        <v>10000</v>
+      </c>
+      <c r="I28" t="n">
+        <v>10000</v>
+      </c>
+      <c r="J28" t="n">
+        <v>408.5628986358643</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>28</v>
+      </c>
+      <c r="B29" t="n">
+        <v>28</v>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>sucrose</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>sucrose</t>
+        </is>
+      </c>
+      <c r="E29" t="n">
+        <v>57</v>
+      </c>
+      <c r="F29" t="n">
+        <v>0</v>
+      </c>
+      <c r="G29" t="n">
+        <v>20000</v>
+      </c>
+      <c r="H29" t="n">
+        <v>10000</v>
+      </c>
+      <c r="I29" t="n">
+        <v>10000</v>
+      </c>
+      <c r="J29" t="n">
+        <v>327.617883682251</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>29</v>
+      </c>
+      <c r="B30" t="n">
+        <v>29</v>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>sucrose</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>sucrose</t>
+        </is>
+      </c>
+      <c r="E30" t="n">
+        <v>0</v>
+      </c>
+      <c r="F30" t="n">
+        <v>0</v>
+      </c>
+      <c r="G30" t="n">
+        <v>20000</v>
+      </c>
+      <c r="H30" t="n">
+        <v>10000</v>
+      </c>
+      <c r="I30" t="n">
+        <v>10000</v>
+      </c>
+      <c r="J30" t="n">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>30</v>
+      </c>
+      <c r="B31" t="n">
+        <v>30</v>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>sucrose</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>sucrose</t>
+        </is>
+      </c>
+      <c r="E31" t="n">
+        <v>0</v>
+      </c>
+      <c r="F31" t="n">
+        <v>55</v>
+      </c>
+      <c r="G31" t="n">
+        <v>20000</v>
+      </c>
+      <c r="H31" t="n">
+        <v>10000</v>
+      </c>
+      <c r="I31" t="n">
+        <v>10000</v>
+      </c>
+      <c r="J31" t="n">
+        <v>4956.228733062744</v>
       </c>
     </row>
   </sheetData>

</xml_diff>